<commit_message>
Added notebooks to create graphs of each dataseries, and to split dataseries from GeoLoket and Vista Datavison
</commit_message>
<xml_diff>
--- a/output_files/data_validation.xlsx
+++ b/output_files/data_validation.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5037,6 +5037,4434 @@
         <v>0</v>
       </c>
     </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B09-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B09-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C171" t="b">
+        <v>0</v>
+      </c>
+      <c r="D171" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E171" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F171" t="n">
+        <v>352</v>
+      </c>
+      <c r="G171" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B09-PB2_m_NAP</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B09-PB2_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C172" t="b">
+        <v>0</v>
+      </c>
+      <c r="D172" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E172" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F172" t="n">
+        <v>352</v>
+      </c>
+      <c r="G172" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B12-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B12-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C173" t="b">
+        <v>0</v>
+      </c>
+      <c r="D173" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E173" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F173" t="n">
+        <v>351</v>
+      </c>
+      <c r="G173" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B13-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B13-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C174" t="b">
+        <v>0</v>
+      </c>
+      <c r="D174" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E174" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F174" t="n">
+        <v>352</v>
+      </c>
+      <c r="G174" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B13-PB2_m_NAP</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B13-PB2_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C175" t="b">
+        <v>0</v>
+      </c>
+      <c r="D175" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E175" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F175" t="n">
+        <v>352</v>
+      </c>
+      <c r="G175" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B14-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B14-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C176" t="b">
+        <v>0</v>
+      </c>
+      <c r="D176" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E176" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F176" t="n">
+        <v>352</v>
+      </c>
+      <c r="G176" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B14-PB2_m_NAP</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B14-PB2_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C177" t="b">
+        <v>0</v>
+      </c>
+      <c r="D177" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E177" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F177" t="n">
+        <v>352</v>
+      </c>
+      <c r="G177" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B15-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B15-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C178" t="b">
+        <v>0</v>
+      </c>
+      <c r="D178" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E178" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F178" t="n">
+        <v>352</v>
+      </c>
+      <c r="G178" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B15-PB2_m_NAP</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B15-PB2_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C179" t="b">
+        <v>0</v>
+      </c>
+      <c r="D179" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E179" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F179" t="n">
+        <v>352</v>
+      </c>
+      <c r="G179" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B16-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B16-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C180" t="b">
+        <v>0</v>
+      </c>
+      <c r="D180" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E180" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F180" t="n">
+        <v>351</v>
+      </c>
+      <c r="G180" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B16-PB2_m_NAP</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B16-PB2_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C181" t="b">
+        <v>0</v>
+      </c>
+      <c r="D181" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E181" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F181" t="n">
+        <v>351</v>
+      </c>
+      <c r="G181" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B17-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B17-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C182" t="b">
+        <v>0</v>
+      </c>
+      <c r="D182" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E182" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F182" t="n">
+        <v>351</v>
+      </c>
+      <c r="G182" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B18-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B18-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C183" t="b">
+        <v>0</v>
+      </c>
+      <c r="D183" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E183" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F183" t="n">
+        <v>351</v>
+      </c>
+      <c r="G183" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B26-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B26-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C184" t="b">
+        <v>0</v>
+      </c>
+      <c r="D184" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E184" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F184" t="n">
+        <v>352</v>
+      </c>
+      <c r="G184" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B26-PB2_m_NAP</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_B26-PB2_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C185" t="b">
+        <v>0</v>
+      </c>
+      <c r="D185" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E185" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F185" t="n">
+        <v>352</v>
+      </c>
+      <c r="G185" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB20-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB20-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C186" t="b">
+        <v>0</v>
+      </c>
+      <c r="D186" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E186" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F186" t="n">
+        <v>351</v>
+      </c>
+      <c r="G186" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB21-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB21-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C187" t="b">
+        <v>0</v>
+      </c>
+      <c r="D187" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E187" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F187" t="n">
+        <v>351</v>
+      </c>
+      <c r="G187" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB22-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB22-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C188" t="b">
+        <v>0</v>
+      </c>
+      <c r="D188" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E188" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F188" t="n">
+        <v>351</v>
+      </c>
+      <c r="G188" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB23-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB23-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C189" t="b">
+        <v>0</v>
+      </c>
+      <c r="D189" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E189" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F189" t="n">
+        <v>352</v>
+      </c>
+      <c r="G189" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB25-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB25-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C190" t="b">
+        <v>0</v>
+      </c>
+      <c r="D190" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E190" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F190" t="n">
+        <v>351</v>
+      </c>
+      <c r="G190" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB27-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB27-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C191" t="b">
+        <v>0</v>
+      </c>
+      <c r="D191" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E191" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F191" t="n">
+        <v>352</v>
+      </c>
+      <c r="G191" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB28-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB28-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C192" t="b">
+        <v>0</v>
+      </c>
+      <c r="D192" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E192" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F192" t="n">
+        <v>351</v>
+      </c>
+      <c r="G192" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB29-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB29-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C193" t="b">
+        <v>0</v>
+      </c>
+      <c r="D193" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E193" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F193" t="n">
+        <v>351</v>
+      </c>
+      <c r="G193" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB30-PB1_m_NAP</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>NL-2412417-HWM_HB30-PB1_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C194" t="b">
+        <v>0</v>
+      </c>
+      <c r="D194" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E194" s="2" t="n">
+        <v>45590</v>
+      </c>
+      <c r="F194" t="n">
+        <v>352</v>
+      </c>
+      <c r="G194" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19092315_B18-PB1_1_53_0_53_m_NAP</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19092315_B18-PB1_1_53_0_53_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C195" t="b">
+        <v>0</v>
+      </c>
+      <c r="D195" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E195" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F195" t="n">
+        <v>607</v>
+      </c>
+      <c r="G195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19103012_B16-PB2_1_6_0_6_m_NAP</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19103012_B16-PB2_1_6_0_6_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C196" t="b">
+        <v>1</v>
+      </c>
+      <c r="D196" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E196" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F196" t="n">
+        <v>607</v>
+      </c>
+      <c r="G196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19120421_HB20-PB1_-2_88_-3_88_m_NAP</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19120421_HB20-PB1_-2_88_-3_88_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C197" t="b">
+        <v>0</v>
+      </c>
+      <c r="D197" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E197" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F197" t="n">
+        <v>607</v>
+      </c>
+      <c r="G197" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19121810_Waterstand_cmH2O</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19121810_Waterstand_cmH2O.csv</t>
+        </is>
+      </c>
+      <c r="C198" t="b">
+        <v>1</v>
+      </c>
+      <c r="D198" s="2" t="n">
+        <v>45621</v>
+      </c>
+      <c r="E198" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F198" t="n">
+        <v>226</v>
+      </c>
+      <c r="G198" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19121817_B15-PB1_-8_97_-9_97_m_NAP</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-19121817_B15-PB1_-8_97_-9_97_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C199" t="b">
+        <v>0</v>
+      </c>
+      <c r="D199" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E199" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F199" t="n">
+        <v>608</v>
+      </c>
+      <c r="G199" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20011012_HB27-PB1_0_16_-0_84_m_NAP</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20011012_HB27-PB1_0_16_-0_84_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C200" t="b">
+        <v>0</v>
+      </c>
+      <c r="D200" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E200" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F200" t="n">
+        <v>608</v>
+      </c>
+      <c r="G200" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20011025_B17-PB1_-3_51_-4_51_m_NAP</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20011025_B17-PB1_-3_51_-4_51_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C201" t="b">
+        <v>0</v>
+      </c>
+      <c r="D201" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E201" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F201" t="n">
+        <v>607</v>
+      </c>
+      <c r="G201" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20030428_HB28-PB1_0_4_-0_6_m_NAP</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20030428_HB28-PB1_0_4_-0_6_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C202" t="b">
+        <v>1</v>
+      </c>
+      <c r="D202" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E202" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F202" t="n">
+        <v>607</v>
+      </c>
+      <c r="G202" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20071684_HB21-PB1_-0_31_-1_31_m_NAP</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20071684_HB21-PB1_-0_31_-1_31_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C203" t="b">
+        <v>1</v>
+      </c>
+      <c r="D203" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E203" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F203" t="n">
+        <v>607</v>
+      </c>
+      <c r="G203" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20111037_HB30-PB1_-5_02_-6_02_m_NAP</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-20111037_HB30-PB1_-5_02_-6_02_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C204" t="b">
+        <v>0</v>
+      </c>
+      <c r="D204" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E204" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F204" t="n">
+        <v>608</v>
+      </c>
+      <c r="G204" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21041455_Waterstand_cmH2O</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21041455_Waterstand_cmH2O.csv</t>
+        </is>
+      </c>
+      <c r="C205" t="b">
+        <v>1</v>
+      </c>
+      <c r="D205" s="2" t="n">
+        <v>45238</v>
+      </c>
+      <c r="E205" s="2" t="n">
+        <v>45641</v>
+      </c>
+      <c r="F205" t="n">
+        <v>404</v>
+      </c>
+      <c r="G205" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21041467_HB22-PB1_-1_4_-2_4_m_NAP</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21041467_HB22-PB1_-1_4_-2_4_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C206" t="b">
+        <v>1</v>
+      </c>
+      <c r="D206" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E206" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F206" t="n">
+        <v>607</v>
+      </c>
+      <c r="G206" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21041468_HB29-PB1_-0_54_-1_54_m_NAP</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21041468_HB29-PB1_-0_54_-1_54_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C207" t="b">
+        <v>1</v>
+      </c>
+      <c r="D207" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E207" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F207" t="n">
+        <v>607</v>
+      </c>
+      <c r="G207" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21052819_HB23-PB1_-0_88_-1_88_m_NAP</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21052819_HB23-PB1_-0_88_-1_88_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C208" t="b">
+        <v>1</v>
+      </c>
+      <c r="D208" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E208" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F208" t="n">
+        <v>608</v>
+      </c>
+      <c r="G208" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21070910_B26-PB2_-1_67_-2_67_m_NAP</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21070910_B26-PB2_-1_67_-2_67_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C209" t="b">
+        <v>0</v>
+      </c>
+      <c r="D209" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E209" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F209" t="n">
+        <v>608</v>
+      </c>
+      <c r="G209" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21070919_HB25-PB1_0_60_-0_39_m_NAP</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21070919_HB25-PB1_0_60_-0_39_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C210" t="b">
+        <v>1</v>
+      </c>
+      <c r="D210" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E210" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F210" t="n">
+        <v>608</v>
+      </c>
+      <c r="G210" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21072016_B12-PB1_0_54_-0_46_m_NAP</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21072016_B12-PB1_0_54_-0_46_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C211" t="b">
+        <v>1</v>
+      </c>
+      <c r="D211" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E211" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F211" t="n">
+        <v>608</v>
+      </c>
+      <c r="G211" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21072702_B09-PB2_-4_22_-5_22_m_NAP</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21072702_B09-PB2_-4_22_-5_22_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C212" t="b">
+        <v>0</v>
+      </c>
+      <c r="D212" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E212" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F212" t="n">
+        <v>608</v>
+      </c>
+      <c r="G212" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21072709_B09-PB1_-14_39_-15_39_m_NAP</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21072709_B09-PB1_-14_39_-15_39_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C213" t="b">
+        <v>0</v>
+      </c>
+      <c r="D213" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E213" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F213" t="n">
+        <v>608</v>
+      </c>
+      <c r="G213" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21093003_B15-PB2_-3_47_-4_47_m_NAP</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21093003_B15-PB2_-3_47_-4_47_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C214" t="b">
+        <v>0</v>
+      </c>
+      <c r="D214" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E214" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F214" t="n">
+        <v>608</v>
+      </c>
+      <c r="G214" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21120911_B14-PB1_-4_95_-5_95_m_NAP</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21120911_B14-PB1_-4_95_-5_95_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C215" t="b">
+        <v>0</v>
+      </c>
+      <c r="D215" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E215" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F215" t="n">
+        <v>608</v>
+      </c>
+      <c r="G215" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21120915_B16-PB1_-6_54_-7_54_m_NAP</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-21120915_B16-PB1_-6_54_-7_54_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C216" t="b">
+        <v>0</v>
+      </c>
+      <c r="D216" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="E216" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F216" t="n">
+        <v>607</v>
+      </c>
+      <c r="G216" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22011103_B14-PB2_0_89_-0_11_m_NAP</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22011103_B14-PB2_0_89_-0_11_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C217" t="b">
+        <v>0</v>
+      </c>
+      <c r="D217" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E217" s="2" t="n">
+        <v>45842</v>
+      </c>
+      <c r="F217" t="n">
+        <v>604</v>
+      </c>
+      <c r="G217" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033010_Waterstand_cmH2O</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033010_Waterstand_cmH2O.csv</t>
+        </is>
+      </c>
+      <c r="C218" t="b">
+        <v>1</v>
+      </c>
+      <c r="D218" s="2" t="n">
+        <v>45253</v>
+      </c>
+      <c r="E218" s="2" t="n">
+        <v>45375</v>
+      </c>
+      <c r="F218" t="n">
+        <v>123</v>
+      </c>
+      <c r="G218" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033032_Waterstand_cmH2O</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033032_Waterstand_cmH2O.csv</t>
+        </is>
+      </c>
+      <c r="C219" t="b">
+        <v>1</v>
+      </c>
+      <c r="D219" s="2" t="n">
+        <v>45238</v>
+      </c>
+      <c r="E219" s="2" t="n">
+        <v>45254</v>
+      </c>
+      <c r="F219" t="n">
+        <v>17</v>
+      </c>
+      <c r="G219" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033044_B26-PB1_-4_82_-5_82_m_NAP</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033044_B26-PB1_-4_82_-5_82_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C220" t="b">
+        <v>0</v>
+      </c>
+      <c r="D220" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E220" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F220" t="n">
+        <v>608</v>
+      </c>
+      <c r="G220" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033049_Waterstand_cmH2O</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22033049_Waterstand_cmH2O.csv</t>
+        </is>
+      </c>
+      <c r="C221" t="b">
+        <v>1</v>
+      </c>
+      <c r="D221" s="2" t="n">
+        <v>45237</v>
+      </c>
+      <c r="E221" s="2" t="n">
+        <v>45254</v>
+      </c>
+      <c r="F221" t="n">
+        <v>18</v>
+      </c>
+      <c r="G221" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22042044_B13-PB1_-9_98_-10_98_m_NAP</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22042044_B13-PB1_-9_98_-10_98_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C222" t="b">
+        <v>0</v>
+      </c>
+      <c r="D222" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E222" s="2" t="n">
+        <v>45844</v>
+      </c>
+      <c r="F222" t="n">
+        <v>606</v>
+      </c>
+      <c r="G222" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22042060_B13-PB2_-3_44_-4_44_m_NAP</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>NL-241417-ET-22042060_B13-PB2_-3_44_-4_44_m_NAP.csv</t>
+        </is>
+      </c>
+      <c r="C223" t="b">
+        <v>0</v>
+      </c>
+      <c r="D223" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="E223" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F223" t="n">
+        <v>608</v>
+      </c>
+      <c r="G223" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-FLB5073_HB-SS060_BIT_PB1_-4_7_-5_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-FLB5073_HB-SS060_BIT_PB1_-4_7_-5_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C224" t="b">
+        <v>0</v>
+      </c>
+      <c r="D224" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E224" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F224" t="n">
+        <v>434</v>
+      </c>
+      <c r="G224" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-FLB5176_HB-SS059_BIT_PB1_-4_3_-5_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-FLB5176_HB-SS059_BIT_PB1_-4_3_-5_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C225" t="b">
+        <v>0</v>
+      </c>
+      <c r="D225" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E225" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F225" t="n">
+        <v>434</v>
+      </c>
+      <c r="G225" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-FLB5207_HB-WM044_KR_PB1_-3_2_-4_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-FLB5207_HB-WM044_KR_PB1_-3_2_-4_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C226" t="b">
+        <v>0</v>
+      </c>
+      <c r="D226" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E226" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F226" t="n">
+        <v>435</v>
+      </c>
+      <c r="G226" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1004_HB-GA035_BIT_PB1_-4_2_-5_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1004_HB-GA035_BIT_PB1_-4_2_-5_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C227" t="b">
+        <v>1</v>
+      </c>
+      <c r="D227" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E227" s="2" t="n">
+        <v>45811</v>
+      </c>
+      <c r="F227" t="n">
+        <v>399</v>
+      </c>
+      <c r="G227" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1064_HB-GA039_BIT_PB1_-3_2_-4_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1064_HB-GA039_BIT_PB1_-3_2_-4_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C228" t="b">
+        <v>1</v>
+      </c>
+      <c r="D228" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E228" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F228" t="n">
+        <v>434</v>
+      </c>
+      <c r="G228" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1083_HB-GA040_BIT_PB1_-3_3_-4_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1083_HB-GA040_BIT_PB1_-3_3_-4_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C229" t="b">
+        <v>0</v>
+      </c>
+      <c r="D229" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E229" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F229" t="n">
+        <v>434</v>
+      </c>
+      <c r="G229" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1112_HB-SS077_BITA_PB1_-3_1_-4_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1112_HB-SS077_BITA_PB1_-3_1_-4_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C230" t="b">
+        <v>0</v>
+      </c>
+      <c r="D230" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E230" s="2" t="n">
+        <v>45827</v>
+      </c>
+      <c r="F230" t="n">
+        <v>415</v>
+      </c>
+      <c r="G230" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1157_HB-GP019_BITA_PB1_-4_3_-5_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1157_HB-GP019_BITA_PB1_-4_3_-5_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C231" t="b">
+        <v>0</v>
+      </c>
+      <c r="D231" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E231" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F231" t="n">
+        <v>436</v>
+      </c>
+      <c r="G231" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1188_PB_SCH3_18_BIT_PB1_-2_5_-3_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1188_PB_SCH3_18_BIT_PB1_-2_5_-3_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C232" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E232" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F232" t="n">
+        <v>436</v>
+      </c>
+      <c r="G232" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1267_HB-GP026_BITA_PB1_-3_1_-4_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1267_HB-GP026_BITA_PB1_-3_1_-4_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C233" t="b">
+        <v>0</v>
+      </c>
+      <c r="D233" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E233" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F233" t="n">
+        <v>435</v>
+      </c>
+      <c r="G233" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1274_HB_GP010_BITA_PB1_-3_7_-4_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1274_HB_GP010_BITA_PB1_-3_7_-4_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C234" t="b">
+        <v>0</v>
+      </c>
+      <c r="D234" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E234" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F234" t="n">
+        <v>436</v>
+      </c>
+      <c r="G234" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1298_PB_SCH3_12_KR_PB1_-0_9_-1_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1298_PB_SCH3_12_KR_PB1_-0_9_-1_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C235" t="b">
+        <v>0</v>
+      </c>
+      <c r="D235" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E235" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="F235" t="n">
+        <v>274</v>
+      </c>
+      <c r="G235" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1303_HB-WM046_AL_PB1_-4_7_-5_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1303_HB-WM046_AL_PB1_-4_7_-5_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C236" t="b">
+        <v>1</v>
+      </c>
+      <c r="D236" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E236" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F236" t="n">
+        <v>435</v>
+      </c>
+      <c r="G236" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1305_HB-SS072_BIT_PB1_-4_1_-5_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1305_HB-SS072_BIT_PB1_-4_1_-5_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C237" t="b">
+        <v>0</v>
+      </c>
+      <c r="D237" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E237" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F237" t="n">
+        <v>435</v>
+      </c>
+      <c r="G237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1326_HB-SS069_BIT_PB1_-2_9_-3_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1326_HB-SS069_BIT_PB1_-2_9_-3_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C238" t="b">
+        <v>1</v>
+      </c>
+      <c r="D238" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E238" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F238" t="n">
+        <v>435</v>
+      </c>
+      <c r="G238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1361_PB_C01_1_KR_PB1_-5_2_-6_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1361_PB_C01_1_KR_PB1_-5_2_-6_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C239" t="b">
+        <v>0</v>
+      </c>
+      <c r="D239" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E239" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F239" t="n">
+        <v>435</v>
+      </c>
+      <c r="G239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1405_PB_SCH3_15_KR_PB1_-1_4_-2_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1405_PB_SCH3_15_KR_PB1_-1_4_-2_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C240" t="b">
+        <v>1</v>
+      </c>
+      <c r="D240" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E240" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F240" t="n">
+        <v>436</v>
+      </c>
+      <c r="G240" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1429_HB-SS061_BIT_PB1_-3_6_-4_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1429_HB-SS061_BIT_PB1_-3_6_-4_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C241" t="b">
+        <v>1</v>
+      </c>
+      <c r="D241" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E241" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F241" t="n">
+        <v>434</v>
+      </c>
+      <c r="G241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1432_PB_SCH3_11_KR_PB1_-0_8_-1_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1432_PB_SCH3_11_KR_PB1_-0_8_-1_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C242" t="b">
+        <v>0</v>
+      </c>
+      <c r="D242" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E242" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F242" t="n">
+        <v>436</v>
+      </c>
+      <c r="G242" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1444_HB-GP015_BITA_PB1_-3_7_-4_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1444_HB-GP015_BITA_PB1_-3_7_-4_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C243" t="b">
+        <v>0</v>
+      </c>
+      <c r="D243" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E243" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F243" t="n">
+        <v>436</v>
+      </c>
+      <c r="G243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1466_PB_SCH3_14_KR_PB1_-0_9_-1_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1466_PB_SCH3_14_KR_PB1_-0_9_-1_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C244" t="b">
+        <v>1</v>
+      </c>
+      <c r="D244" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E244" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F244" t="n">
+        <v>436</v>
+      </c>
+      <c r="G244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1513_HB-GP024_BITA_PB1_-3_9_-4_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1513_HB-GP024_BITA_PB1_-3_9_-4_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C245" t="b">
+        <v>0</v>
+      </c>
+      <c r="D245" s="2" t="n">
+        <v>45411</v>
+      </c>
+      <c r="E245" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F245" t="n">
+        <v>436</v>
+      </c>
+      <c r="G245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1603_HB-SS059_BIT_PB1_-4_3_-5_3_-_Copy_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1603_HB-SS059_BIT_PB1_-4_3_-5_3_-_Copy_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C246" t="b">
+        <v>0</v>
+      </c>
+      <c r="D246" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E246" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F246" t="n">
+        <v>93</v>
+      </c>
+      <c r="G246" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1603_HB-SS059_BIT_PB1_-4_3_-5_3_-_Copy_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1603_HB-SS059_BIT_PB1_-4_3_-5_3_-_Copy_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C247" t="b">
+        <v>0</v>
+      </c>
+      <c r="D247" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="E247" s="2" t="n">
+        <v>45505</v>
+      </c>
+      <c r="F247" t="n">
+        <v>93</v>
+      </c>
+      <c r="G247" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1605_HB-GA029_KR_PB1_-3_4_-4_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB1605_HB-GA029_KR_PB1_-3_4_-4_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C248" t="b">
+        <v>0</v>
+      </c>
+      <c r="D248" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E248" s="2" t="n">
+        <v>45837</v>
+      </c>
+      <c r="F248" t="n">
+        <v>426</v>
+      </c>
+      <c r="G248" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB5127_PB_C01_2_KR_PB1_-5_4_-6_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>NL-253677-FB-LB5127_PB_C01_2_KR_PB1_-5_4_-6_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C249" t="b">
+        <v>0</v>
+      </c>
+      <c r="D249" s="2" t="n">
+        <v>45412</v>
+      </c>
+      <c r="E249" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F249" t="n">
+        <v>435</v>
+      </c>
+      <c r="G249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5014_HB11PB01_-2_0_-3_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5014_HB11PB01_-2_0_-3_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C250" t="b">
+        <v>0</v>
+      </c>
+      <c r="D250" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E250" s="2" t="n">
+        <v>45839</v>
+      </c>
+      <c r="F250" t="n">
+        <v>169</v>
+      </c>
+      <c r="G250" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5017_B26PB01_-6_7_-7_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5017_B26PB01_-6_7_-7_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C251" t="b">
+        <v>0</v>
+      </c>
+      <c r="D251" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E251" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F251" t="n">
+        <v>161</v>
+      </c>
+      <c r="G251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5017_B26PB02_-3_2_-4_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5017_B26PB02_-3_2_-4_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C252" t="b">
+        <v>0</v>
+      </c>
+      <c r="D252" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E252" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F252" t="n">
+        <v>161</v>
+      </c>
+      <c r="G252" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5022_HB16PB01_-3_2_-4_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5022_HB16PB01_-3_2_-4_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C253" t="b">
+        <v>1</v>
+      </c>
+      <c r="D253" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E253" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F253" t="n">
+        <v>170</v>
+      </c>
+      <c r="G253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5026_HB19PB01_-2_5_-3_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5026_HB19PB01_-2_5_-3_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C254" t="b">
+        <v>0</v>
+      </c>
+      <c r="D254" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E254" s="2" t="n">
+        <v>45845</v>
+      </c>
+      <c r="F254" t="n">
+        <v>169</v>
+      </c>
+      <c r="G254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5032_HB22PB01_-3_6_-4_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5032_HB22PB01_-3_6_-4_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C255" t="b">
+        <v>0</v>
+      </c>
+      <c r="D255" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E255" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F255" t="n">
+        <v>162</v>
+      </c>
+      <c r="G255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5033_B19PB01_-5_8_-6_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5033_B19PB01_-5_8_-6_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C256" t="b">
+        <v>0</v>
+      </c>
+      <c r="D256" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E256" s="2" t="n">
+        <v>45843</v>
+      </c>
+      <c r="F256" t="n">
+        <v>167</v>
+      </c>
+      <c r="G256" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5033_B19PB02_-3_8_-4_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5033_B19PB02_-3_8_-4_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C257" t="b">
+        <v>0</v>
+      </c>
+      <c r="D257" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E257" s="2" t="n">
+        <v>45843</v>
+      </c>
+      <c r="F257" t="n">
+        <v>167</v>
+      </c>
+      <c r="G257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5044_HB26PB01_-3_3_-4_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5044_HB26PB01_-3_3_-4_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C258" t="b">
+        <v>0</v>
+      </c>
+      <c r="D258" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E258" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F258" t="n">
+        <v>161</v>
+      </c>
+      <c r="G258" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5045_B02PB01_-4_1_-5_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5045_B02PB01_-4_1_-5_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C259" t="b">
+        <v>0</v>
+      </c>
+      <c r="D259" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E259" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F259" t="n">
+        <v>181</v>
+      </c>
+      <c r="G259" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5045_B02PB02_-2_2_-3_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5045_B02PB02_-2_2_-3_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C260" t="b">
+        <v>0</v>
+      </c>
+      <c r="D260" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E260" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F260" t="n">
+        <v>181</v>
+      </c>
+      <c r="G260" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5047_HB06PB01_-2_8_-3_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5047_HB06PB01_-2_8_-3_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C261" t="b">
+        <v>0</v>
+      </c>
+      <c r="D261" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E261" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F261" t="n">
+        <v>176</v>
+      </c>
+      <c r="G261" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5049_B17PB01_-5_2_-6_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5049_B17PB01_-5_2_-6_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C262" t="b">
+        <v>0</v>
+      </c>
+      <c r="D262" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E262" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F262" t="n">
+        <v>169</v>
+      </c>
+      <c r="G262" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5049_B17PB02_-2_7_-3_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5049_B17PB02_-2_7_-3_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C263" t="b">
+        <v>0</v>
+      </c>
+      <c r="D263" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E263" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F263" t="n">
+        <v>169</v>
+      </c>
+      <c r="G263" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5050_HB02PB01_-2_2_-3_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5050_HB02PB01_-2_2_-3_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C264" t="b">
+        <v>0</v>
+      </c>
+      <c r="D264" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E264" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F264" t="n">
+        <v>181</v>
+      </c>
+      <c r="G264" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5052_B15PB01_-5_1_-6_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5052_B15PB01_-5_1_-6_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C265" t="b">
+        <v>0</v>
+      </c>
+      <c r="D265" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E265" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F265" t="n">
+        <v>161</v>
+      </c>
+      <c r="G265" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5052_B15PB02_-3_1_-4_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5052_B15PB02_-3_1_-4_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C266" t="b">
+        <v>0</v>
+      </c>
+      <c r="D266" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E266" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F266" t="n">
+        <v>161</v>
+      </c>
+      <c r="G266" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5059_HB25PB01_-5_4_-6_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5059_HB25PB01_-5_4_-6_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C267" t="b">
+        <v>0</v>
+      </c>
+      <c r="D267" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E267" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F267" t="n">
+        <v>162</v>
+      </c>
+      <c r="G267" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5061_B05PB01_-6_0_-7_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5061_B05PB01_-6_0_-7_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C268" t="b">
+        <v>0</v>
+      </c>
+      <c r="D268" s="2" t="n">
+        <v>45667</v>
+      </c>
+      <c r="E268" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F268" t="n">
+        <v>180</v>
+      </c>
+      <c r="G268" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5061_B05PB02_-1_2_-2_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5061_B05PB02_-1_2_-2_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C269" t="b">
+        <v>0</v>
+      </c>
+      <c r="D269" s="2" t="n">
+        <v>45667</v>
+      </c>
+      <c r="E269" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F269" t="n">
+        <v>180</v>
+      </c>
+      <c r="G269" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5069_HB01PB01_-1_9_-2_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5069_HB01PB01_-1_9_-2_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C270" t="b">
+        <v>0</v>
+      </c>
+      <c r="D270" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E270" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F270" t="n">
+        <v>181</v>
+      </c>
+      <c r="G270" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5070_HB14PB01_-3_8_-4_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5070_HB14PB01_-3_8_-4_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C271" t="b">
+        <v>0</v>
+      </c>
+      <c r="D271" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E271" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F271" t="n">
+        <v>162</v>
+      </c>
+      <c r="G271" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5079_B01PB01_-3_6_-4_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5079_B01PB01_-3_6_-4_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C272" t="b">
+        <v>0</v>
+      </c>
+      <c r="D272" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E272" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F272" t="n">
+        <v>181</v>
+      </c>
+      <c r="G272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5079_B01PB02_-0_6_-1_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5079_B01PB02_-0_6_-1_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C273" t="b">
+        <v>1</v>
+      </c>
+      <c r="D273" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E273" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F273" t="n">
+        <v>181</v>
+      </c>
+      <c r="G273" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5083_B03PB01_-5_0_-6_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5083_B03PB01_-5_0_-6_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C274" t="b">
+        <v>0</v>
+      </c>
+      <c r="D274" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E274" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F274" t="n">
+        <v>181</v>
+      </c>
+      <c r="G274" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5083_B03PB02_-0_5_-1_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5083_B03PB02_-0_5_-1_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C275" t="b">
+        <v>1</v>
+      </c>
+      <c r="D275" s="2" t="n">
+        <v>45666</v>
+      </c>
+      <c r="E275" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F275" t="n">
+        <v>181</v>
+      </c>
+      <c r="G275" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5086_B10PB01_-4_2_-5_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5086_B10PB01_-4_2_-5_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C276" t="b">
+        <v>0</v>
+      </c>
+      <c r="D276" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E276" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F276" t="n">
+        <v>176</v>
+      </c>
+      <c r="G276" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5086_B10PB02_-2_4_-3_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5086_B10PB02_-2_4_-3_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C277" t="b">
+        <v>0</v>
+      </c>
+      <c r="D277" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E277" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F277" t="n">
+        <v>176</v>
+      </c>
+      <c r="G277" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5088_B07PB01_-1_9_-2_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5088_B07PB01_-1_9_-2_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C278" t="b">
+        <v>0</v>
+      </c>
+      <c r="D278" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E278" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F278" t="n">
+        <v>162</v>
+      </c>
+      <c r="G278" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5091_HB27PB01_-3_4_-4_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5091_HB27PB01_-3_4_-4_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C279" t="b">
+        <v>0</v>
+      </c>
+      <c r="D279" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E279" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F279" t="n">
+        <v>161</v>
+      </c>
+      <c r="G279" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5092_B16PB01_-5_6_-6_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5092_B16PB01_-5_6_-6_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C280" t="b">
+        <v>0</v>
+      </c>
+      <c r="D280" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E280" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F280" t="n">
+        <v>169</v>
+      </c>
+      <c r="G280" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5092_B16PB02_-3_0_-4_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5092_B16PB02_-3_0_-4_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C281" t="b">
+        <v>0</v>
+      </c>
+      <c r="D281" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E281" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F281" t="n">
+        <v>169</v>
+      </c>
+      <c r="G281" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5094_HB31PB01_-3_0_-4_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5094_HB31PB01_-3_0_-4_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C282" t="b">
+        <v>0</v>
+      </c>
+      <c r="D282" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E282" s="2" t="n">
+        <v>45827</v>
+      </c>
+      <c r="F282" t="n">
+        <v>142</v>
+      </c>
+      <c r="G282" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5099_HB13PB01_-2_1_-3_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5099_HB13PB01_-2_1_-3_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C283" t="b">
+        <v>1</v>
+      </c>
+      <c r="D283" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E283" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F283" t="n">
+        <v>160</v>
+      </c>
+      <c r="G283" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5103_HB15PB01_-2_9_-3_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5103_HB15PB01_-2_9_-3_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C284" t="b">
+        <v>0</v>
+      </c>
+      <c r="D284" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E284" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F284" t="n">
+        <v>169</v>
+      </c>
+      <c r="G284" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5105_B18PB01_-6_5_-7_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5105_B18PB01_-6_5_-7_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C285" t="b">
+        <v>0</v>
+      </c>
+      <c r="D285" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E285" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F285" t="n">
+        <v>160</v>
+      </c>
+      <c r="G285" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5105_B18PB02_-2_1_-3_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5105_B18PB02_-2_1_-3_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C286" t="b">
+        <v>1</v>
+      </c>
+      <c r="D286" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E286" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F286" t="n">
+        <v>160</v>
+      </c>
+      <c r="G286" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5106_B22PB01_-7_4_-8_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5106_B22PB01_-7_4_-8_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C287" t="b">
+        <v>0</v>
+      </c>
+      <c r="D287" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E287" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F287" t="n">
+        <v>170</v>
+      </c>
+      <c r="G287" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5106_B22PB02_-4_5_-5_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5106_B22PB02_-4_5_-5_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C288" t="b">
+        <v>0</v>
+      </c>
+      <c r="D288" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E288" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F288" t="n">
+        <v>170</v>
+      </c>
+      <c r="G288" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5125_B11PB01_-3_6_-4_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5125_B11PB01_-3_6_-4_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C289" t="b">
+        <v>0</v>
+      </c>
+      <c r="D289" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E289" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F289" t="n">
+        <v>176</v>
+      </c>
+      <c r="G289" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5125_B11PB02_-2_4_-3_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5125_B11PB02_-2_4_-3_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C290" t="b">
+        <v>0</v>
+      </c>
+      <c r="D290" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E290" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F290" t="n">
+        <v>176</v>
+      </c>
+      <c r="G290" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5128_B20PB01_-11_5_-12_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5128_B20PB01_-11_5_-12_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C291" t="b">
+        <v>0</v>
+      </c>
+      <c r="D291" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E291" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F291" t="n">
+        <v>170</v>
+      </c>
+      <c r="G291" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5128_B20PB02_-3_2_-4_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5128_B20PB02_-3_2_-4_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C292" t="b">
+        <v>0</v>
+      </c>
+      <c r="D292" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E292" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F292" t="n">
+        <v>170</v>
+      </c>
+      <c r="G292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5132_HB12PB01_-3_7_-4_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5132_HB12PB01_-3_7_-4_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C293" t="b">
+        <v>0</v>
+      </c>
+      <c r="D293" s="2" t="n">
+        <v>45671</v>
+      </c>
+      <c r="E293" s="2" t="n">
+        <v>45845</v>
+      </c>
+      <c r="F293" t="n">
+        <v>175</v>
+      </c>
+      <c r="G293" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5134_HB21PB01_-5_7_-6_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5134_HB21PB01_-5_7_-6_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C294" t="b">
+        <v>0</v>
+      </c>
+      <c r="D294" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="E294" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F294" t="n">
+        <v>163</v>
+      </c>
+      <c r="G294" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5146_HB23PB01_-3_8_-4_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5146_HB23PB01_-3_8_-4_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C295" t="b">
+        <v>0</v>
+      </c>
+      <c r="D295" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E295" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F295" t="n">
+        <v>161</v>
+      </c>
+      <c r="G295" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5147_HB32PB01_-4_5_-5_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5147_HB32PB01_-4_5_-5_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C296" t="b">
+        <v>0</v>
+      </c>
+      <c r="D296" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E296" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F296" t="n">
+        <v>161</v>
+      </c>
+      <c r="G296" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5149_B06PB01_-7_5_-8_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5149_B06PB01_-7_5_-8_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C297" t="b">
+        <v>0</v>
+      </c>
+      <c r="D297" s="2" t="n">
+        <v>45667</v>
+      </c>
+      <c r="E297" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F297" t="n">
+        <v>180</v>
+      </c>
+      <c r="G297" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5149_B06PB02_-2_7_-3_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5149_B06PB02_-2_7_-3_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C298" t="b">
+        <v>0</v>
+      </c>
+      <c r="D298" s="2" t="n">
+        <v>45667</v>
+      </c>
+      <c r="E298" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F298" t="n">
+        <v>180</v>
+      </c>
+      <c r="G298" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5151_HB24PB01_-3_4_-4_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5151_HB24PB01_-3_4_-4_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C299" t="b">
+        <v>0</v>
+      </c>
+      <c r="D299" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E299" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F299" t="n">
+        <v>162</v>
+      </c>
+      <c r="G299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5154_B13PB01_-4_8_-5_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5154_B13PB01_-4_8_-5_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C300" t="b">
+        <v>0</v>
+      </c>
+      <c r="D300" s="2" t="n">
+        <v>45672</v>
+      </c>
+      <c r="E300" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F300" t="n">
+        <v>175</v>
+      </c>
+      <c r="G300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5154_B13PB02_-0_7_-1_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5154_B13PB02_-0_7_-1_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C301" t="b">
+        <v>0</v>
+      </c>
+      <c r="D301" s="2" t="n">
+        <v>45672</v>
+      </c>
+      <c r="E301" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F301" t="n">
+        <v>175</v>
+      </c>
+      <c r="G301" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5157_B30PB01_-5_2_-6_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5157_B30PB01_-5_2_-6_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C302" t="b">
+        <v>0</v>
+      </c>
+      <c r="D302" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="E302" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F302" t="n">
+        <v>163</v>
+      </c>
+      <c r="G302" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5157_B30PB02_-3_7_-4_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5157_B30PB02_-3_7_-4_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C303" t="b">
+        <v>0</v>
+      </c>
+      <c r="D303" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="E303" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F303" t="n">
+        <v>161</v>
+      </c>
+      <c r="G303" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5159_B12PB01_-7_0_-8_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5159_B12PB01_-7_0_-8_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C304" t="b">
+        <v>0</v>
+      </c>
+      <c r="D304" s="2" t="n">
+        <v>45672</v>
+      </c>
+      <c r="E304" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F304" t="n">
+        <v>175</v>
+      </c>
+      <c r="G304" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5159_B12PB02_-2_9_-3_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5159_B12PB02_-2_9_-3_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C305" t="b">
+        <v>0</v>
+      </c>
+      <c r="D305" s="2" t="n">
+        <v>45672</v>
+      </c>
+      <c r="E305" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F305" t="n">
+        <v>175</v>
+      </c>
+      <c r="G305" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5165_B25PB01_-6_9_-7_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5165_B25PB01_-6_9_-7_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C306" t="b">
+        <v>0</v>
+      </c>
+      <c r="D306" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E306" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F306" t="n">
+        <v>162</v>
+      </c>
+      <c r="G306" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5165_B25PB02_-4_0_-5_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5165_B25PB02_-4_0_-5_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C307" t="b">
+        <v>0</v>
+      </c>
+      <c r="D307" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E307" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F307" t="n">
+        <v>162</v>
+      </c>
+      <c r="G307" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5177_B29PB01_-13_1_-14_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5177_B29PB01_-13_1_-14_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C308" t="b">
+        <v>0</v>
+      </c>
+      <c r="D308" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E308" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F308" t="n">
+        <v>160</v>
+      </c>
+      <c r="G308" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5177_B29PB02_-3_9_-4_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5177_B29PB02_-3_9_-4_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C309" t="b">
+        <v>0</v>
+      </c>
+      <c r="D309" s="2" t="n">
+        <v>45098</v>
+      </c>
+      <c r="E309" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F309" t="n">
+        <v>749</v>
+      </c>
+      <c r="G309" t="n">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5182_HB18PB01_-3_2_-4_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5182_HB18PB01_-3_2_-4_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C310" t="b">
+        <v>0</v>
+      </c>
+      <c r="D310" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E310" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F310" t="n">
+        <v>160</v>
+      </c>
+      <c r="G310" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5185_B24PB01_-8_0_-9_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5185_B24PB01_-8_0_-9_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C311" t="b">
+        <v>0</v>
+      </c>
+      <c r="D311" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E311" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F311" t="n">
+        <v>162</v>
+      </c>
+      <c r="G311" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5185_B24PB02_-3_5_-4_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5185_B24PB02_-3_5_-4_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C312" t="b">
+        <v>0</v>
+      </c>
+      <c r="D312" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E312" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F312" t="n">
+        <v>162</v>
+      </c>
+      <c r="G312" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5190_B23PB01_-3_8_-4_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5190_B23PB01_-3_8_-4_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C313" t="b">
+        <v>0</v>
+      </c>
+      <c r="D313" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E313" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F313" t="n">
+        <v>169</v>
+      </c>
+      <c r="G313" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5190_B23PB02_0_0_-1_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5190_B23PB02_0_0_-1_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C314" t="b">
+        <v>0</v>
+      </c>
+      <c r="D314" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E314" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F314" t="n">
+        <v>169</v>
+      </c>
+      <c r="G314" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5199_B21PB01_-5_5_-6_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5199_B21PB01_-5_5_-6_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C315" t="b">
+        <v>0</v>
+      </c>
+      <c r="D315" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E315" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F315" t="n">
+        <v>160</v>
+      </c>
+      <c r="G315" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5200_B14PB01_-3_9_-4_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5200_B14PB01_-3_9_-4_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C316" t="b">
+        <v>0</v>
+      </c>
+      <c r="D316" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E316" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F316" t="n">
+        <v>170</v>
+      </c>
+      <c r="G316" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5200_B14PB02_-1_5_-2_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5200_B14PB02_-1_5_-2_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C317" t="b">
+        <v>0</v>
+      </c>
+      <c r="D317" s="2" t="n">
+        <v>45677</v>
+      </c>
+      <c r="E317" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F317" t="n">
+        <v>170</v>
+      </c>
+      <c r="G317" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5203_B04PB01_-5_4_-6_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5203_B04PB01_-5_4_-6_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C318" t="b">
+        <v>0</v>
+      </c>
+      <c r="D318" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="E318" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F318" t="n">
+        <v>162</v>
+      </c>
+      <c r="G318" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5298_HB17PB01_-3_6_-4_6_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5298_HB17PB01_-3_6_-4_6_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C319" t="b">
+        <v>0</v>
+      </c>
+      <c r="D319" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="E319" s="2" t="n">
+        <v>45845</v>
+      </c>
+      <c r="F319" t="n">
+        <v>159</v>
+      </c>
+      <c r="G319" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5336_HB03PB01_-1_3_-2_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>NL-260484-FB-FLB5336_HB03PB01_-1_3_-2_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C320" t="b">
+        <v>0</v>
+      </c>
+      <c r="D320" s="2" t="n">
+        <v>45678</v>
+      </c>
+      <c r="E320" s="2" t="n">
+        <v>45845</v>
+      </c>
+      <c r="F320" t="n">
+        <v>168</v>
+      </c>
+      <c r="G320" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5029_B09PB01_-7_1_-8_1_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5029_B09PB01_-7_1_-8_1_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C321" t="b">
+        <v>0</v>
+      </c>
+      <c r="D321" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E321" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F321" t="n">
+        <v>208</v>
+      </c>
+      <c r="G321" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5029_B09PB02_-2_3_-3_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5029_B09PB02_-2_3_-3_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C322" t="b">
+        <v>0</v>
+      </c>
+      <c r="D322" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E322" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F322" t="n">
+        <v>208</v>
+      </c>
+      <c r="G322" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5036_B08PB01_-5_0_-6_0_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5036_B08PB01_-5_0_-6_0_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C323" t="b">
+        <v>0</v>
+      </c>
+      <c r="D323" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E323" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F323" t="n">
+        <v>208</v>
+      </c>
+      <c r="G323" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5036_B08PB02_-1_4_-2_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5036_B08PB02_-1_4_-2_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C324" t="b">
+        <v>1</v>
+      </c>
+      <c r="D324" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E324" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F324" t="n">
+        <v>208</v>
+      </c>
+      <c r="G324" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5055_HB02PB01_-1_5_-2_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5055_HB02PB01_-1_5_-2_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C325" t="b">
+        <v>0</v>
+      </c>
+      <c r="D325" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E325" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F325" t="n">
+        <v>208</v>
+      </c>
+      <c r="G325" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5082_B04PB01_-2_2_-3_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5082_B04PB01_-2_2_-3_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C326" t="b">
+        <v>0</v>
+      </c>
+      <c r="D326" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E326" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F326" t="n">
+        <v>208</v>
+      </c>
+      <c r="G326" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5085_B03PB01_-2_3_-3_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5085_B03PB01_-2_3_-3_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C327" t="b">
+        <v>0</v>
+      </c>
+      <c r="D327" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E327" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F327" t="n">
+        <v>208</v>
+      </c>
+      <c r="G327" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5093_HB01PB01_-2_7_-3_7_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5093_HB01PB01_-2_7_-3_7_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C328" t="b">
+        <v>0</v>
+      </c>
+      <c r="D328" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E328" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F328" t="n">
+        <v>208</v>
+      </c>
+      <c r="G328" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5095_B07PB01_-1_2_-2_2_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5095_B07PB01_-1_2_-2_2_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C329" t="b">
+        <v>0</v>
+      </c>
+      <c r="D329" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E329" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F329" t="n">
+        <v>208</v>
+      </c>
+      <c r="G329" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5140_B10PB01_-0_3_-1_3_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5140_B10PB01_-0_3_-1_3_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C330" t="b">
+        <v>0</v>
+      </c>
+      <c r="D330" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E330" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F330" t="n">
+        <v>208</v>
+      </c>
+      <c r="G330" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5141_B11PB01_-4_8_-5_8_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5141_B11PB01_-4_8_-5_8_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C331" t="b">
+        <v>0</v>
+      </c>
+      <c r="D331" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E331" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F331" t="n">
+        <v>208</v>
+      </c>
+      <c r="G331" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5141_B11PB02_-2_4_-3_4_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5141_B11PB02_-2_4_-3_4_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C332" t="b">
+        <v>0</v>
+      </c>
+      <c r="D332" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E332" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F332" t="n">
+        <v>208</v>
+      </c>
+      <c r="G332" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5153_HB03PB01_-1_9_-2_9_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5153_HB03PB01_-1_9_-2_9_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C333" t="b">
+        <v>1</v>
+      </c>
+      <c r="D333" s="2" t="n">
+        <v>45639</v>
+      </c>
+      <c r="E333" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F333" t="n">
+        <v>208</v>
+      </c>
+      <c r="G333" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5163_B07aPB2_-5_5_-6_5_m_NAP_avg</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>NL-263591-FB-FLB5163_B07aPB2_-5_5_-6_5_m_NAP_avg.csv</t>
+        </is>
+      </c>
+      <c r="C334" t="b">
+        <v>0</v>
+      </c>
+      <c r="D334" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="E334" s="2" t="n">
+        <v>45846</v>
+      </c>
+      <c r="F334" t="n">
+        <v>159</v>
+      </c>
+      <c r="G334" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>